<commit_message>
better noise standard deviation
have updated the method to get standard deviation of noise so that it can be calculated in one pass, rather than using a big array of floats. also accounted for erroneous values and forced a rate on the measurements
</commit_message>
<xml_diff>
--- a/PDC/helperFiles/testsAndTodo.xlsx
+++ b/PDC/helperFiles/testsAndTodo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rory\Documents\Uni_and_otherWork\Jobs etc\UoS_SunSat\Avionics-Code-for-Arduino-\PDC\helperFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCE94AA-5A90-4FB4-8D21-5F0B4B4FC914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EA0152-19BA-4425-BDCC-B2609E244FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A28AD64C-69C9-40DF-90AD-FA585136F58E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>A list of tests and tasks. Some require hardware, some require discussion w/ relevant people</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Discussion</t>
+  </si>
+  <si>
+    <t>replace errFlag with an 8 bit (?) binary code where each bit indicates a different error?</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF1C8F3-9A76-496E-81FD-ABC3D29924E7}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,6 +697,20 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added gyroscope setup and read functions
</commit_message>
<xml_diff>
--- a/PDC/helperFiles/testsAndTodo.xlsx
+++ b/PDC/helperFiles/testsAndTodo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rory\Documents\Uni_and_otherWork\Jobs etc\UoS_SunSat\Avionics-Code-for-Arduino-\PDC\helperFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16323D87-B533-40BB-9AFA-64942C34EEDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4876CBCE-E303-427F-A401-0DB9C6605C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A28AD64C-69C9-40DF-90AD-FA585136F58E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>A list of tests and tasks. Some require hardware, some require discussion w/ relevant people</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>does readI2C() return values as expected?</t>
+  </si>
+  <si>
+    <t>refactor IMU reading (i.e. methods like read.gyro.z())</t>
   </si>
 </sst>
 </file>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF1C8F3-9A76-496E-81FD-ABC3D29924E7}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,6 +771,20 @@
       </c>
       <c r="D17" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commenting and cleaning up
changed some formatting to be more consistent, have addressed some TODOs, added new items to the test spreadsheet, and generally cleaned up a bit
</commit_message>
<xml_diff>
--- a/PDC/helperFiles/testsAndTodo.xlsx
+++ b/PDC/helperFiles/testsAndTodo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rory\Documents\Uni_and_otherWork\Jobs etc\UoS_SunSat\Avionics-Code-for-Arduino-\PDC\helperFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F218A9AD-F082-4A54-A4D8-CF2B6FF33918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5975B1F-B3B4-433C-999D-AB2433E82B03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A28AD64C-69C9-40DF-90AD-FA585136F58E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>A list of tests and tasks. Some require hardware, some require discussion w/ relevant people</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>look at replacing LPA with single sensor w/ intensity readout (analog?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in accel init, maybe measure noise at different ranges so we can switch mid flight </t>
+  </si>
+  <si>
+    <t>does the altimeter temp/press/alt match the expected values?</t>
+  </si>
+  <si>
+    <t>develop error/status codes that can be written to 'notes' in log file (strings are expensive)</t>
   </si>
 </sst>
 </file>
@@ -541,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF1C8F3-9A76-496E-81FD-ABC3D29924E7}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +763,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -768,7 +777,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -886,6 +895,48 @@
         <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>